<commit_message>
arreglo excel líneas teóricas de acuerdo con velocidad
</commit_message>
<xml_diff>
--- a/Espectro completo de arturo_visualizador/Espectro completo de arturo_visualizador/lineas_teoricas_hierro1.xlsx
+++ b/Espectro completo de arturo_visualizador/Espectro completo de arturo_visualizador/lineas_teoricas_hierro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessi Dani\OneDrive - Universidad de los andes\Proyecto Teórico\Proyecto-Te-rico-Arturo\Espectro completo de arturo_visualizador\Espectro completo de arturo_visualizador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A52403-4F06-463F-A784-A68A6F3E7DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19216BE-EEEE-4F81-9494-8D9C2988292C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A801"/>
+  <dimension ref="A1:A800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,3016 +1378,3011 @@
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>4942.4592000000002</v>
+        <v>4945.6373999999996</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>4945.6373999999996</v>
+        <v>4946.3881000000001</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>4946.3881000000001</v>
+        <v>4950.1059999999998</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>4950.1059999999998</v>
+        <v>4962.5718999999999</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>4962.5718999999999</v>
+        <v>4966.0888999999997</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>4966.0888999999997</v>
+        <v>4967.8973999999998</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>4967.8973999999998</v>
+        <v>4969.9175999999998</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>4969.9175999999998</v>
+        <v>4970.4957999999997</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>4970.4957999999997</v>
+        <v>4982.4998999999998</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>4982.4998999999998</v>
+        <v>4983.2506999999996</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>4983.2506999999996</v>
+        <v>4983.8528999999999</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>4983.8528999999999</v>
+        <v>4985.2529000000004</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211">
-        <v>4985.2529000000004</v>
+        <v>4985.5473000000002</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>4985.5473000000002</v>
+        <v>4986.2226000000001</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>4986.2226000000001</v>
+        <v>4988.9501</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>4988.9501</v>
+        <v>4994.1295</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>4994.1295</v>
+        <v>4999.1125000000002</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>4999.1125000000002</v>
+        <v>5001.8635999999997</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>5001.8635999999997</v>
+        <v>5002.7927</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>5002.7927</v>
+        <v>5004.0442999999996</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>5004.0442999999996</v>
+        <v>5005.7123000000001</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>5005.7123000000001</v>
+        <v>5006.1190999999999</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>5006.1190999999999</v>
+        <v>5014.9425000000001</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>5014.9425000000001</v>
+        <v>5022.2354999999998</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>5022.2354999999998</v>
+        <v>5023.1866</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>5023.1866</v>
+        <v>5027.7566999999999</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>5027.7566999999999</v>
+        <v>5028.1264000000001</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>5028.1264000000001</v>
+        <v>5029.6175999999996</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>5029.6175999999996</v>
+        <v>5030.7785999999996</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>5030.7785999999996</v>
+        <v>5044.2114000000001</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>5044.2114000000001</v>
+        <v>5049.8198000000002</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>5049.8198000000002</v>
+        <v>5054.6426000000001</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>5054.6426000000001</v>
+        <v>5060.0789999999997</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>5060.0789999999997</v>
+        <v>5067.1495999999997</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>5067.1495999999997</v>
+        <v>5068.7658000000001</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>5068.7658000000001</v>
+        <v>5072.0784000000003</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>5072.0784000000003</v>
+        <v>5072.6720999999998</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>5072.6720999999998</v>
+        <v>5074.7483000000002</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>5074.7483000000002</v>
+        <v>5076.2646000000004</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>5076.2646000000004</v>
+        <v>5078.9748</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>5078.9748</v>
+        <v>5079.223</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>5079.223</v>
+        <v>5079.74</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>5079.74</v>
+        <v>5083.3386</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>5083.3386</v>
+        <v>5090.7740000000003</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>5090.7740000000003</v>
+        <v>5096.9979999999996</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>5096.9979999999996</v>
+        <v>5099.0772999999999</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>5099.0772999999999</v>
+        <v>5109.652</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>5109.652</v>
+        <v>5115.7781000000004</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247">
-        <v>5115.7781000000004</v>
+        <v>5123.72</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>5123.72</v>
+        <v>5127.3593000000001</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>5127.3593000000001</v>
+        <v>5131.4687000000004</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>5131.4687000000004</v>
+        <v>5133.6885000000002</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>5133.6885000000002</v>
+        <v>5137.3822</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>5137.3822</v>
+        <v>5141.7389999999996</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>5141.7389999999996</v>
+        <v>5148.0428000000002</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>5148.0428000000002</v>
+        <v>5148.2291999999998</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>5148.2291999999998</v>
+        <v>5150.8395</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>5150.8395</v>
+        <v>5159.0576000000001</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>5159.0576000000001</v>
+        <v>5162.2728999999999</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>5162.2728999999999</v>
+        <v>5166.2821999999996</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>5166.2821999999996</v>
+        <v>5187.9142000000002</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260">
-        <v>5187.9142000000002</v>
+        <v>5194.9417999999996</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>5194.9417999999996</v>
+        <v>5195.4723000000004</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262">
-        <v>5195.4723000000004</v>
+        <v>5196.0595999999996</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>5196.0595999999996</v>
+        <v>5198.7111000000004</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264">
-        <v>5198.7111000000004</v>
+        <v>5215.1805999999997</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>5215.1805999999997</v>
+        <v>5216.2740000000003</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>5216.2740000000003</v>
+        <v>5217.3892999999998</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>5217.3892999999998</v>
+        <v>5223.1854999999996</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>5223.1854999999996</v>
+        <v>5225.5261</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>5225.5261</v>
+        <v>5226.0661</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>5226.0661</v>
+        <v>5226.8622999999998</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>5226.8622999999998</v>
+        <v>5228.3766999999998</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272">
-        <v>5228.3766999999998</v>
+        <v>5232.9403000000002</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>5232.9403000000002</v>
+        <v>5242.4911000000002</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>5242.4911000000002</v>
+        <v>5243.7768999999998</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>5243.7768999999998</v>
+        <v>5247.0504000000001</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>5247.0504000000001</v>
+        <v>5250.2088999999996</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>5250.2088999999996</v>
+        <v>5250.6459999999997</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278">
-        <v>5250.6459999999997</v>
+        <v>5253.4616999999998</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>5253.4616999999998</v>
+        <v>5263.3063000000002</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>5263.3063000000002</v>
+        <v>5263.8649999999998</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281">
-        <v>5263.8649999999998</v>
+        <v>5266.5554000000002</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282">
-        <v>5266.5554000000002</v>
+        <v>5269.5374000000002</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283">
-        <v>5269.5374000000002</v>
+        <v>5270.3563999999997</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284">
-        <v>5270.3563999999997</v>
+        <v>5273.1635999999999</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285">
-        <v>5273.1635999999999</v>
+        <v>5273.3735999999999</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>5273.3735999999999</v>
+        <v>5281.7903999999999</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>5281.7903999999999</v>
+        <v>5283.6210000000001</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288">
-        <v>5283.6210000000001</v>
+        <v>5288.5246999999999</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>5288.5246999999999</v>
+        <v>5298.7758000000003</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290">
-        <v>5298.7758000000003</v>
+        <v>5307.3609999999999</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>5307.3609999999999</v>
+        <v>5322.0407999999998</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292">
-        <v>5322.0407999999998</v>
+        <v>5324.1790000000001</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293">
-        <v>5324.1790000000001</v>
+        <v>5326.1427999999996</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294">
-        <v>5326.1427999999996</v>
+        <v>5329.9890999999998</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>5329.9890999999998</v>
+        <v>5332.8996999999999</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296">
-        <v>5332.8996999999999</v>
+        <v>5339.9294</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>5339.9294</v>
+        <v>5341.0240000000003</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298">
-        <v>5341.0240000000003</v>
+        <v>5349.7376000000004</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299">
-        <v>5349.7376000000004</v>
+        <v>5364.8712999999998</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300">
-        <v>5364.8712999999998</v>
+        <v>5365.3990999999996</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301">
-        <v>5365.3990999999996</v>
+        <v>5369.9619000000002</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302">
-        <v>5369.9619000000002</v>
+        <v>5371.4897000000001</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303">
-        <v>5371.4897000000001</v>
+        <v>5373.7085999999999</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304">
-        <v>5373.7085999999999</v>
+        <v>5379.5739999999996</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>5379.5739999999996</v>
+        <v>5383.3692000000001</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306">
-        <v>5383.3692000000001</v>
+        <v>5389.4791999999998</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307">
-        <v>5389.4791999999998</v>
+        <v>5393.1675999999998</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308">
-        <v>5393.1675999999998</v>
+        <v>5397.1279999999997</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>5397.1279999999997</v>
+        <v>5397.6178</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310">
-        <v>5397.6178</v>
+        <v>5398.2794000000004</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311">
-        <v>5398.2794000000004</v>
+        <v>5403.8215</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312">
-        <v>5403.8215</v>
+        <v>5405.7752</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313">
-        <v>5405.7752</v>
+        <v>5409.1336000000001</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314">
-        <v>5409.1336000000001</v>
+        <v>5410.9098000000004</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
-        <v>5410.9098000000004</v>
+        <v>5415.1993000000002</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316">
-        <v>5415.1993000000002</v>
+        <v>5424.0681999999997</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
-        <v>5424.0681999999997</v>
+        <v>5432.9479000000001</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318">
-        <v>5432.9479000000001</v>
+        <v>5434.5237999999999</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319">
-        <v>5434.5237999999999</v>
+        <v>5445.0424000000003</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320">
-        <v>5445.0424000000003</v>
+        <v>5446.5829000000003</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321">
-        <v>5446.5829000000003</v>
+        <v>5462.9594999999999</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322">
-        <v>5462.9594999999999</v>
+        <v>5463.2762000000002</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323">
-        <v>5463.2762000000002</v>
+        <v>5464.2795999999998</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324">
-        <v>5464.2795999999998</v>
+        <v>5466.3962000000001</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325">
-        <v>5466.3962000000001</v>
+        <v>5466.9877999999999</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326">
-        <v>5466.9877999999999</v>
+        <v>5472.7091</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327">
-        <v>5472.7091</v>
+        <v>5473.9004999999997</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328">
-        <v>5473.9004999999997</v>
+        <v>5476.2884999999997</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329">
-        <v>5476.2884999999997</v>
+        <v>5476.5641999999998</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330">
-        <v>5476.5641999999998</v>
+        <v>5483.0987999999998</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331">
-        <v>5483.0987999999998</v>
+        <v>5487.7460000000001</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332">
-        <v>5487.7460000000001</v>
+        <v>5493.4988000000003</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333">
-        <v>5493.4988000000003</v>
+        <v>5497.5160999999998</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334">
-        <v>5497.5160999999998</v>
+        <v>5501.4652999999998</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335">
-        <v>5501.4652999999998</v>
+        <v>5506.7790999999997</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336">
-        <v>5506.7790999999997</v>
+        <v>5522.4465</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337">
-        <v>5522.4465</v>
+        <v>5525.5442999999996</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338">
-        <v>5525.5442999999996</v>
+        <v>5543.1895999999997</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339">
-        <v>5543.1895999999997</v>
+        <v>5543.9357</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340">
-        <v>5543.9357</v>
+        <v>5546.5057999999999</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341">
-        <v>5546.5057999999999</v>
+        <v>5554.8950999999997</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342">
-        <v>5554.8950999999997</v>
+        <v>5560.2115999999996</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343">
-        <v>5560.2115999999996</v>
+        <v>5562.7065000000002</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344">
-        <v>5562.7065000000002</v>
+        <v>5565.7039999999997</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345">
-        <v>5565.7039999999997</v>
+        <v>5567.3910999999998</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346">
-        <v>5567.3910999999998</v>
+        <v>5569.6180999999997</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347">
-        <v>5569.6180999999997</v>
+        <v>5572.8424000000005</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348">
-        <v>5572.8424000000005</v>
+        <v>5576.0888000000004</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349">
-        <v>5576.0888000000004</v>
+        <v>5584.7646999999997</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350">
-        <v>5584.7646999999997</v>
+        <v>5586.7559000000001</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351">
-        <v>5586.7559000000001</v>
+        <v>5587.5739999999996</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352">
-        <v>5587.5739999999996</v>
+        <v>5600.2241999999997</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353">
-        <v>5600.2241999999997</v>
+        <v>5615.2965999999997</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354">
-        <v>5615.2965999999997</v>
+        <v>5615.6439</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355">
-        <v>5615.6439</v>
+        <v>5618.6327000000001</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356">
-        <v>5618.6327000000001</v>
+        <v>5619.5954000000002</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357">
-        <v>5619.5954000000002</v>
+        <v>5620.4924000000001</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358">
-        <v>5620.4924000000001</v>
+        <v>5624.0219999999999</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359">
-        <v>5624.0219999999999</v>
+        <v>5624.5421999999999</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360">
-        <v>5624.5421999999999</v>
+        <v>5633.9465</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361">
-        <v>5633.9465</v>
+        <v>5635.8226000000004</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362">
-        <v>5635.8226000000004</v>
+        <v>5636.6962000000003</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363">
-        <v>5636.6962000000003</v>
+        <v>5637.1081000000004</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364">
-        <v>5637.1081000000004</v>
+        <v>5638.2620999999999</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365">
-        <v>5638.2620999999999</v>
+        <v>5645.8338000000003</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366">
-        <v>5645.8338000000003</v>
+        <v>5649.9872999999998</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367">
-        <v>5649.9872999999998</v>
+        <v>5651.4690000000001</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368">
-        <v>5651.4690000000001</v>
+        <v>5652.3180000000002</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369">
-        <v>5652.3180000000002</v>
+        <v>5653.8667999999998</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370">
-        <v>5653.8667999999998</v>
+        <v>5655.1764999999996</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371">
-        <v>5655.1764999999996</v>
+        <v>5655.49</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372">
-        <v>5655.49</v>
+        <v>5659.5747000000001</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373">
-        <v>5659.5747000000001</v>
+        <v>5660.8010999999997</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374">
-        <v>5660.8010999999997</v>
+        <v>5661.3455000000004</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375">
-        <v>5661.3455000000004</v>
+        <v>5662.5162</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376">
-        <v>5662.5162</v>
+        <v>5667.518</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377">
-        <v>5667.518</v>
+        <v>5677.6848</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378">
-        <v>5677.6848</v>
+        <v>5678.3788000000004</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379">
-        <v>5678.3788000000004</v>
+        <v>5679.0228999999999</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380">
-        <v>5679.0228999999999</v>
+        <v>5680.2403999999997</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381">
-        <v>5680.2403999999997</v>
+        <v>5686.5302000000001</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382">
-        <v>5686.5302000000001</v>
+        <v>5691.4970000000003</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383">
-        <v>5691.4970000000003</v>
+        <v>5696.0896000000002</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384">
-        <v>5696.0896000000002</v>
+        <v>5698.02</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385">
-        <v>5698.02</v>
+        <v>5701.5446000000002</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386">
-        <v>5701.5446000000002</v>
+        <v>5704.7336999999998</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
-        <v>5704.7336999999998</v>
+        <v>5705.4646000000002</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388">
-        <v>5705.4646000000002</v>
+        <v>5709.9323000000004</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389">
-        <v>5709.9323000000004</v>
+        <v>5712.1315999999997</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390">
-        <v>5712.1315999999997</v>
+        <v>5714.5491000000002</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391">
-        <v>5714.5491000000002</v>
+        <v>5717.8329000000003</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392">
-        <v>5717.8329000000003</v>
+        <v>5720.8981999999996</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
-        <v>5720.8981999999996</v>
+        <v>5724.4547000000002</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394">
-        <v>5724.4547000000002</v>
+        <v>5731.7623000000003</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
-        <v>5731.7623000000003</v>
+        <v>5732.2960000000003</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396">
-        <v>5732.2960000000003</v>
+        <v>5734.5652</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
-        <v>5734.5652</v>
+        <v>5738.2277000000004</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398">
-        <v>5738.2277000000004</v>
+        <v>5741.8483999999999</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
-        <v>5741.8483999999999</v>
+        <v>5742.96</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400">
-        <v>5742.96</v>
+        <v>5752.0320000000002</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401">
-        <v>5752.0320000000002</v>
+        <v>5753.1226999999999</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402">
-        <v>5753.1226999999999</v>
+        <v>5754.4026000000003</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403">
-        <v>5754.4026000000003</v>
+        <v>5759.2620999999999</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404">
-        <v>5759.2620999999999</v>
+        <v>5759.5411999999997</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405">
-        <v>5759.5411999999997</v>
+        <v>5760.3446000000004</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406">
-        <v>5760.3446000000004</v>
+        <v>5762.9921999999997</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407">
-        <v>5762.9921999999997</v>
+        <v>5769.3227999999999</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408">
-        <v>5769.3227999999999</v>
+        <v>5775.0806000000002</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409">
-        <v>5775.0806000000002</v>
+        <v>5776.2244000000001</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410">
-        <v>5776.2244000000001</v>
+        <v>5780.6000999999997</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411">
-        <v>5780.6000999999997</v>
+        <v>5780.8042999999998</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412">
-        <v>5780.8042999999998</v>
+        <v>5782.1095999999998</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413">
-        <v>5782.1095999999998</v>
+        <v>5784.6584000000003</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414">
-        <v>5784.6584000000003</v>
+        <v>5791.5239000000001</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415">
-        <v>5791.5239000000001</v>
+        <v>5793.9147999999996</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416">
-        <v>5793.9147999999996</v>
+        <v>5798.1714000000002</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417">
-        <v>5798.1714000000002</v>
+        <v>5804.0349999999999</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418">
-        <v>5804.0349999999999</v>
+        <v>5805.7570999999998</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419">
-        <v>5805.7570999999998</v>
+        <v>5806.7249000000002</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420">
-        <v>5806.7249000000002</v>
+        <v>5807.7838000000002</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421">
-        <v>5807.7838000000002</v>
+        <v>5811.9144999999999</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422">
-        <v>5811.9144999999999</v>
+        <v>5814.8074999999999</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423">
-        <v>5814.8074999999999</v>
+        <v>5817.0765000000001</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424">
-        <v>5817.0765000000001</v>
+        <v>5827.8770999999997</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425">
-        <v>5827.8770999999997</v>
+        <v>5835.1008000000002</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426">
-        <v>5835.1008000000002</v>
+        <v>5835.5735000000004</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427">
-        <v>5835.5735000000004</v>
+        <v>5837.7012000000004</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428">
-        <v>5837.7012000000004</v>
+        <v>5838.3717999999999</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429">
-        <v>5838.3717999999999</v>
+        <v>5844.9188000000004</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430">
-        <v>5844.9188000000004</v>
+        <v>5845.2869000000001</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431">
-        <v>5845.2869000000001</v>
+        <v>5849.1850000000004</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432">
-        <v>5849.1850000000004</v>
+        <v>5849.6840000000002</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433">
-        <v>5849.6840000000002</v>
+        <v>5851.2052000000003</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434">
-        <v>5851.2052000000003</v>
+        <v>5853.1482999999998</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435">
-        <v>5853.1482999999998</v>
+        <v>5853.6826000000001</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436">
-        <v>5853.6826000000001</v>
+        <v>5855.0766000000003</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437">
-        <v>5855.0766000000003</v>
+        <v>5856.0879999999997</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438">
-        <v>5856.0879999999997</v>
+        <v>5858.2654000000002</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439">
-        <v>5858.2654000000002</v>
+        <v>5858.7780000000002</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440">
-        <v>5858.7780000000002</v>
+        <v>5859.5866999999998</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441">
-        <v>5859.5866999999998</v>
+        <v>5861.1095999999998</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442">
-        <v>5861.1095999999998</v>
+        <v>5862.3564999999999</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443">
-        <v>5862.3564999999999</v>
+        <v>5864.2443999999996</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444">
-        <v>5864.2443999999996</v>
+        <v>5871.3037000000004</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445">
-        <v>5871.3037000000004</v>
+        <v>5873.2129000000004</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446">
-        <v>5873.2129000000004</v>
+        <v>5876.2781999999997</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447">
-        <v>5876.2781999999997</v>
+        <v>5880.0272000000004</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448">
-        <v>5880.0272000000004</v>
+        <v>5881.2800999999999</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449">
-        <v>5881.2800999999999</v>
+        <v>5883.817</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450">
-        <v>5883.817</v>
+        <v>5891.1759000000002</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451">
-        <v>5891.1759000000002</v>
+        <v>5898.2152999999998</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452">
-        <v>5898.2152999999998</v>
+        <v>5901.5313999999998</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453">
-        <v>5901.5313999999998</v>
+        <v>5902.4736000000003</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454">
-        <v>5902.4736000000003</v>
+        <v>5905.6719999999996</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455">
-        <v>5905.6719999999996</v>
+        <v>5906.8429999999998</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456">
-        <v>5906.8429999999998</v>
+        <v>5907.8634000000002</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457">
-        <v>5907.8634000000002</v>
+        <v>5909.9736000000003</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458">
-        <v>5909.9736000000003</v>
+        <v>5916.2474000000002</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459">
-        <v>5916.2474000000002</v>
+        <v>5927.7891</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A460">
-        <v>5927.7891</v>
+        <v>5929.6772000000001</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461">
-        <v>5929.6772000000001</v>
+        <v>5930.1799000000001</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A462">
-        <v>5930.1799000000001</v>
+        <v>5934.6549000000005</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463">
-        <v>5934.6549000000005</v>
+        <v>5940.9915000000001</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A464">
-        <v>5940.9915000000001</v>
+        <v>5943.5784000000003</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A465">
-        <v>5943.5784000000003</v>
+        <v>5947.5114999999996</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A466">
-        <v>5947.5114999999996</v>
+        <v>5952.7183999999997</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A467">
-        <v>5952.7183999999997</v>
+        <v>5956.6944000000003</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A468">
-        <v>5956.6944000000003</v>
+        <v>5963.2385999999997</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469">
-        <v>5963.2385999999997</v>
+        <v>5969.5622000000003</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A470">
-        <v>5969.5622000000003</v>
+        <v>5976.1603999999998</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471">
-        <v>5976.1603999999998</v>
+        <v>5976.4390999999996</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A472">
-        <v>5976.4390999999996</v>
+        <v>5976.7771000000002</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473">
-        <v>5976.7771000000002</v>
+        <v>5983.6809999999996</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A474">
-        <v>5983.6809999999996</v>
+        <v>5984.8150999999998</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A475">
-        <v>5984.8150999999998</v>
+        <v>5987.0649000000003</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A476">
-        <v>5987.0649000000003</v>
+        <v>5997.7777999999998</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A477">
-        <v>5997.7777999999998</v>
+        <v>6003.0123000000003</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A478">
-        <v>6003.0123000000003</v>
+        <v>6005.5412999999999</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A479">
-        <v>6005.5412999999999</v>
+        <v>6007.9601000000002</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A480">
-        <v>6007.9601000000002</v>
+        <v>6008.5565999999999</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481">
-        <v>6008.5565999999999</v>
+        <v>6012.2098999999998</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482">
-        <v>6012.2098999999998</v>
+        <v>6015.2443000000003</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A483">
-        <v>6015.2443000000003</v>
+        <v>6019.3658999999998</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A484">
-        <v>6019.3658999999998</v>
+        <v>6021.7911999999997</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485">
-        <v>6021.7911999999997</v>
+        <v>6024.058</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A486">
-        <v>6024.058</v>
+        <v>6027.0509000000002</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487">
-        <v>6027.0509000000002</v>
+        <v>6034.0355</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A488">
-        <v>6034.0355</v>
+        <v>6054.0740999999998</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A489">
-        <v>6054.0740999999998</v>
+        <v>6056.0047000000004</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A490">
-        <v>6056.0047000000004</v>
+        <v>6060.6243000000004</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491">
-        <v>6060.6243000000004</v>
+        <v>6062.8483999999999</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A492">
-        <v>6062.8483999999999</v>
+        <v>6078.4911000000002</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493">
-        <v>6078.4911000000002</v>
+        <v>6079.0092999999997</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A494">
-        <v>6079.0092999999997</v>
+        <v>6082.7106000000003</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495">
-        <v>6082.7106000000003</v>
+        <v>6085.259</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A496">
-        <v>6085.259</v>
+        <v>6093.6444000000001</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497">
-        <v>6093.6444000000001</v>
+        <v>6094.3735999999999</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A498">
-        <v>6094.3735999999999</v>
+        <v>6096.6652999999997</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499">
-        <v>6096.6652999999997</v>
+        <v>6098.2447000000002</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A500">
-        <v>6098.2447000000002</v>
+        <v>6100.2716</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501">
-        <v>6100.2716</v>
+        <v>6102.1777000000002</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502">
-        <v>6102.1777000000002</v>
+        <v>6105.1314000000002</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A503">
-        <v>6105.1314000000002</v>
+        <v>6120.2493999999997</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A504">
-        <v>6120.2493999999997</v>
+        <v>6127.9066000000003</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A505">
-        <v>6127.9066000000003</v>
+        <v>6136.6153000000004</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A506">
-        <v>6136.6153000000004</v>
+        <v>6136.9947000000002</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A507">
-        <v>6136.9947000000002</v>
+        <v>6137.6917000000003</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A508">
-        <v>6137.6917000000003</v>
+        <v>6141.732</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A509">
-        <v>6141.732</v>
+        <v>6151.6180999999997</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A510">
-        <v>6151.6180999999997</v>
+        <v>6157.7284</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A511">
-        <v>6157.7284</v>
+        <v>6163.5445</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A512">
-        <v>6163.5445</v>
+        <v>6165.3603000000003</v>
       </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A513">
-        <v>6165.3603000000003</v>
+        <v>6173.3356000000003</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A514">
-        <v>6173.3356000000003</v>
+        <v>6180.2042000000001</v>
       </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A515">
-        <v>6180.2042000000001</v>
+        <v>6187.9903999999997</v>
       </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A516">
-        <v>6187.9903999999997</v>
+        <v>6200.3128999999999</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A517">
-        <v>6200.3128999999999</v>
+        <v>6213.4303</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A518">
-        <v>6213.4303</v>
+        <v>6219.2809999999999</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A519">
-        <v>6219.2809999999999</v>
+        <v>6232.6412</v>
       </c>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A520">
-        <v>6232.6412</v>
+        <v>6240.6462000000001</v>
       </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A521">
-        <v>6240.6462000000001</v>
+        <v>6246.3188</v>
       </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A522">
-        <v>6246.3188</v>
+        <v>6252.5554000000002</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A523">
-        <v>6252.5554000000002</v>
+        <v>6254.2584999999999</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A524">
-        <v>6254.2584999999999</v>
+        <v>6256.3615</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A525">
-        <v>6256.3615</v>
+        <v>6265.134</v>
       </c>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A526">
-        <v>6265.134</v>
+        <v>6270.2250000000004</v>
       </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A527">
-        <v>6270.2250000000004</v>
+        <v>6280.6181999999999</v>
       </c>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A528">
-        <v>6280.6181999999999</v>
+        <v>6290.9656000000004</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A529">
-        <v>6290.9656000000004</v>
+        <v>6297.7930999999999</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A530">
-        <v>6297.7930999999999</v>
+        <v>6301.5011999999997</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A531">
-        <v>6301.5011999999997</v>
+        <v>6302.4935999999998</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A532">
-        <v>6302.4935999999998</v>
+        <v>6311.5002999999997</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A533">
-        <v>6311.5002999999997</v>
+        <v>6315.8114999999998</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A534">
-        <v>6315.8114999999998</v>
+        <v>6318.0174999999999</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A535">
-        <v>6318.0174999999999</v>
+        <v>6322.6854999999996</v>
       </c>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A536">
-        <v>6322.6854999999996</v>
+        <v>6330.8495000000003</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A537">
-        <v>6330.8495000000003</v>
+        <v>6335.3307999999997</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A538">
-        <v>6335.3307999999997</v>
+        <v>6336.8243000000002</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A539">
-        <v>6336.8243000000002</v>
+        <v>6338.8774999999996</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A540">
-        <v>6338.8774999999996</v>
+        <v>6344.1490999999996</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A541">
-        <v>6344.1490999999996</v>
+        <v>6355.0290000000005</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A542">
-        <v>6355.0290000000005</v>
+        <v>6362.8762999999999</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A543">
-        <v>6362.8762999999999</v>
+        <v>6380.7433000000001</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A544">
-        <v>6380.7433000000001</v>
+        <v>6385.7184999999999</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A545">
-        <v>6385.7184999999999</v>
+        <v>6392.5388000000003</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A546">
-        <v>6392.5388000000003</v>
+        <v>6393.6013000000003</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A547">
-        <v>6393.6013000000003</v>
+        <v>6400.0011999999997</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A548">
-        <v>6400.0011999999997</v>
+        <v>6400.3180000000002</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A549">
-        <v>6400.3180000000002</v>
+        <v>6408.0183999999999</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A550">
-        <v>6408.0183999999999</v>
+        <v>6411.6493</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A551">
-        <v>6411.6493</v>
+        <v>6419.6454000000003</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A552">
-        <v>6419.6454000000003</v>
+        <v>6419.9495999999999</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A553">
-        <v>6419.9495999999999</v>
+        <v>6430.8464000000004</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A554">
-        <v>6430.8464000000004</v>
+        <v>6436.4071999999996</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A555">
-        <v>6436.4071999999996</v>
+        <v>6464.6642000000002</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A556">
-        <v>6464.6642000000002</v>
+        <v>6475.6243999999997</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A557">
-        <v>6475.6243999999997</v>
+        <v>6481.8702999999996</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A558">
-        <v>6481.8702999999996</v>
+        <v>6494.4998999999998</v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A559">
-        <v>6494.4998999999998</v>
+        <v>6494.9804999999997</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A560">
-        <v>6494.9804999999997</v>
+        <v>6495.7421999999997</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A561">
-        <v>6495.7421999999997</v>
+        <v>6496.4665999999997</v>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A562">
-        <v>6496.4665999999997</v>
+        <v>6498.9391999999998</v>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A563">
-        <v>6498.9391999999998</v>
+        <v>6504.1835000000001</v>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A564">
-        <v>6504.1835000000001</v>
+        <v>6509.6167999999998</v>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A565">
-        <v>6509.6167999999998</v>
+        <v>6518.3671000000004</v>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A566">
-        <v>6518.3671000000004</v>
+        <v>6533.9294</v>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A567">
-        <v>6533.9294</v>
+        <v>6538.4939000000004</v>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A568">
-        <v>6538.4939000000004</v>
+        <v>6546.2394999999997</v>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A569">
-        <v>6546.2394999999997</v>
+        <v>6551.6779999999999</v>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A570">
-        <v>6551.6779999999999</v>
+        <v>6556.7879999999996</v>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A571">
-        <v>6556.7879999999996</v>
+        <v>6569.2155000000002</v>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A572">
-        <v>6569.2155000000002</v>
+        <v>6575.0158000000001</v>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A573">
-        <v>6575.0158000000001</v>
+        <v>6581.2101000000002</v>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A574">
-        <v>6581.2101000000002</v>
+        <v>6591.3128999999999</v>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A575">
-        <v>6591.3128999999999</v>
+        <v>6592.9138000000003</v>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A576">
-        <v>6592.9138000000003</v>
+        <v>6593.8705</v>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A577">
-        <v>6593.8705</v>
+        <v>6597.5610999999999</v>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A578">
-        <v>6597.5610999999999</v>
+        <v>6604.5889999999999</v>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A579">
-        <v>6604.5889999999999</v>
+        <v>6608.0259999999998</v>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A580">
-        <v>6608.0259999999998</v>
+        <v>6609.1103000000003</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A581">
-        <v>6609.1103000000003</v>
+        <v>6613.8253999999997</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A582">
-        <v>6613.8253999999997</v>
+        <v>6625.0219999999999</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A583">
-        <v>6625.0219999999999</v>
+        <v>6627.5447999999997</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A584">
-        <v>6627.5447999999997</v>
+        <v>6633.4125000000004</v>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A585">
-        <v>6633.4125000000004</v>
+        <v>6633.7497000000003</v>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A586">
-        <v>6633.7497000000003</v>
+        <v>6634.1071000000002</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A587">
-        <v>6634.1071000000002</v>
+        <v>6646.9318000000003</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A588">
-        <v>6646.9318000000003</v>
+        <v>6648.0810000000001</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A589">
-        <v>6648.0810000000001</v>
+        <v>6653.8527000000004</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A590">
-        <v>6653.8527000000004</v>
+        <v>6663.4421000000002</v>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A591">
-        <v>6663.4421000000002</v>
+        <v>6667.4191000000001</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A592">
-        <v>6667.4191000000001</v>
+        <v>6667.7112999999999</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A593">
-        <v>6667.7112999999999</v>
+        <v>6677.9870000000001</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A594">
-        <v>6677.9870000000001</v>
+        <v>6692.2723999999998</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A595">
-        <v>6692.2723999999998</v>
+        <v>6699.1418000000003</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A596">
-        <v>6699.1418000000003</v>
+        <v>6703.5673999999999</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A597">
-        <v>6703.5673999999999</v>
+        <v>6704.4808999999996</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A598">
-        <v>6704.4808999999996</v>
+        <v>6705.1023999999998</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A599">
-        <v>6705.1023999999998</v>
+        <v>6707.4332000000004</v>
       </c>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A600">
-        <v>6707.4332000000004</v>
+        <v>6710.3194999999996</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A601">
-        <v>6710.3194999999996</v>
+        <v>6713.7448000000004</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A602">
-        <v>6713.7448000000004</v>
+        <v>6715.3832000000002</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A603">
-        <v>6715.3832000000002</v>
+        <v>6725.3572000000004</v>
       </c>
     </row>
     <row r="604" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A604">
-        <v>6725.3572000000004</v>
+        <v>6726.6668</v>
       </c>
     </row>
     <row r="605" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A605">
-        <v>6726.6668</v>
+        <v>6730.2924000000003</v>
       </c>
     </row>
     <row r="606" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A606">
-        <v>6730.2924000000003</v>
+        <v>6732.0649000000003</v>
       </c>
     </row>
     <row r="607" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A607">
-        <v>6732.0649000000003</v>
+        <v>6733.1513000000004</v>
       </c>
     </row>
     <row r="608" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A608">
-        <v>6733.1513000000004</v>
+        <v>6737.9870000000001</v>
       </c>
     </row>
     <row r="609" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A609">
-        <v>6737.9870000000001</v>
+        <v>6739.5218999999997</v>
       </c>
     </row>
     <row r="610" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A610">
-        <v>6739.5218999999997</v>
+        <v>6745.1013000000003</v>
       </c>
     </row>
     <row r="611" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A611">
-        <v>6745.1013000000003</v>
+        <v>6745.9565000000002</v>
       </c>
     </row>
     <row r="612" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A612">
-        <v>6745.9565000000002</v>
+        <v>6746.9548999999997</v>
       </c>
     </row>
     <row r="613" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A613">
-        <v>6746.9548999999997</v>
+        <v>6750.1525000000001</v>
       </c>
     </row>
     <row r="614" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A614">
-        <v>6750.1525000000001</v>
+        <v>6752.7070999999996</v>
       </c>
     </row>
     <row r="615" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A615">
-        <v>6752.7070999999996</v>
+        <v>6753.4638999999997</v>
       </c>
     </row>
     <row r="616" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A616">
-        <v>6753.4638999999997</v>
+        <v>6777.4093999999996</v>
       </c>
     </row>
     <row r="617" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A617">
-        <v>6777.4093999999996</v>
+        <v>6783.7039000000004</v>
       </c>
     </row>
     <row r="618" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A618">
-        <v>6783.7039000000004</v>
+        <v>6786.4268000000002</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A619">
-        <v>6786.4268000000002</v>
+        <v>6786.8603999999996</v>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A620">
-        <v>6786.8603999999996</v>
+        <v>6793.2592000000004</v>
       </c>
     </row>
     <row r="621" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A621">
-        <v>6793.2592000000004</v>
+        <v>6804.0009</v>
       </c>
     </row>
     <row r="622" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A622">
-        <v>6804.0009</v>
+        <v>6804.2713000000003</v>
       </c>
     </row>
     <row r="623" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A623">
-        <v>6804.2713000000003</v>
+        <v>6806.8449000000001</v>
       </c>
     </row>
     <row r="624" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A624">
-        <v>6806.8449000000001</v>
+        <v>6810.2628000000004</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A625">
-        <v>6810.2628000000004</v>
+        <v>6820.3719000000001</v>
       </c>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A626">
-        <v>6820.3719000000001</v>
+        <v>6828.5911999999998</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A627">
-        <v>6828.5911999999998</v>
+        <v>6837.0060999999996</v>
       </c>
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A628">
-        <v>6837.0060999999996</v>
+        <v>6839.8305</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A629">
-        <v>6839.8305</v>
+        <v>6842.6858000000002</v>
       </c>
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A630">
-        <v>6842.6858000000002</v>
+        <v>6843.6559999999999</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A631">
-        <v>6843.6559999999999</v>
+        <v>6855.1620999999996</v>
       </c>
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A632">
-        <v>6855.1620999999996</v>
+        <v>6857.2502999999997</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A633">
-        <v>6857.2502999999997</v>
+        <v>6858.1498000000001</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A634">
-        <v>6858.1498000000001</v>
+        <v>6916.6814999999997</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A635">
-        <v>6916.6814999999997</v>
+        <v>6945.2052000000003</v>
       </c>
     </row>
     <row r="636" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A636">
-        <v>6945.2052000000003</v>
+        <v>6978.8516</v>
       </c>
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A637">
-        <v>6978.8516</v>
+        <v>6999.8841000000002</v>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A638">
-        <v>6999.8841000000002</v>
+        <v>7022.9539000000004</v>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A639">
-        <v>7022.9539000000004</v>
+        <v>7038.2233999999999</v>
       </c>
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A640">
-        <v>7038.2233999999999</v>
+        <v>7090.3834999999999</v>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A641">
-        <v>7090.3834999999999</v>
+        <v>7130.9220999999998</v>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A642">
-        <v>7130.9220999999998</v>
+        <v>7132.9862999999996</v>
       </c>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A643">
-        <v>7132.9862999999996</v>
+        <v>7164.4485999999997</v>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A644">
-        <v>7164.4485999999997</v>
+        <v>7181.1958999999997</v>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A645">
-        <v>7181.1958999999997</v>
+        <v>7187.3180000000002</v>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A646">
-        <v>7187.3180000000002</v>
+        <v>7207.1116000000002</v>
       </c>
     </row>
     <row r="647" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A647">
-        <v>7207.1116000000002</v>
+        <v>7207.3879999999999</v>
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A648">
-        <v>7207.3879999999999</v>
+        <v>7288.7385000000004</v>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A649">
-        <v>7288.7385000000004</v>
+        <v>7307.9318000000003</v>
       </c>
     </row>
     <row r="650" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A650">
-        <v>7307.9318000000003</v>
+        <v>7311.0758999999998</v>
       </c>
     </row>
     <row r="651" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A651">
-        <v>7311.0758999999998</v>
+        <v>7389.3987999999999</v>
       </c>
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A652">
-        <v>7389.3987999999999</v>
+        <v>7401.6849000000002</v>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A653">
-        <v>7401.6849000000002</v>
+        <v>7411.1544000000004</v>
       </c>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A654">
-        <v>7411.1544000000004</v>
+        <v>7418.6674000000003</v>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A655">
-        <v>7418.6674000000003</v>
+        <v>7430.8567000000003</v>
       </c>
     </row>
     <row r="656" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A656">
-        <v>7430.8567000000003</v>
+        <v>7440.9121999999998</v>
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A657">
-        <v>7440.9121999999998</v>
+        <v>7443.0223999999998</v>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A658">
-        <v>7443.0223999999998</v>
+        <v>7445.7507999999998</v>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A659">
-        <v>7445.7507999999998</v>
+        <v>7447.3937999999998</v>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A660">
-        <v>7447.3937999999998</v>
+        <v>7461.5205999999998</v>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A661">
-        <v>7461.5205999999998</v>
+        <v>7473.5538999999999</v>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A662">
-        <v>7473.5538999999999</v>
+        <v>7491.6486000000004</v>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A663">
-        <v>7491.6486000000004</v>
+        <v>7495.0673999999999</v>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A664">
-        <v>7495.0673999999999</v>
+        <v>7507.2663000000002</v>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A665">
-        <v>7507.2663000000002</v>
+        <v>7511.0204999999996</v>
       </c>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A666">
-        <v>7511.0204999999996</v>
+        <v>7531.1450999999997</v>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A667">
-        <v>7531.1450999999997</v>
+        <v>7541.9128000000001</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A668">
-        <v>7541.9128000000001</v>
+        <v>7547.8968000000004</v>
       </c>
     </row>
     <row r="669" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A669">
-        <v>7547.8968000000004</v>
+        <v>7559.72</v>
       </c>
     </row>
     <row r="670" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A670">
-        <v>7559.72</v>
+        <v>7563.0108</v>
       </c>
     </row>
     <row r="671" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A671">
-        <v>7563.0108</v>
+        <v>7568.8999000000003</v>
       </c>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A672">
-        <v>7568.8999000000003</v>
+        <v>7582.1219000000001</v>
       </c>
     </row>
     <row r="673" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A673">
-        <v>7582.1219000000001</v>
+        <v>7583.7882</v>
       </c>
     </row>
     <row r="674" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A674">
-        <v>7583.7882</v>
+        <v>7586.0186999999996</v>
       </c>
     </row>
     <row r="675" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A675">
-        <v>7586.0186999999996</v>
+        <v>7588.3053</v>
       </c>
     </row>
     <row r="676" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A676">
-        <v>7588.3053</v>
+        <v>7617.9897000000001</v>
       </c>
     </row>
     <row r="677" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A677">
-        <v>7617.9897000000001</v>
+        <v>7620.5128000000004</v>
       </c>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A678">
-        <v>7620.5128000000004</v>
+        <v>7653.7596000000003</v>
       </c>
     </row>
     <row r="679" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A679">
-        <v>7653.7596000000003</v>
+        <v>7664.2933000000003</v>
       </c>
     </row>
     <row r="680" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A680">
-        <v>7664.2933000000003</v>
+        <v>7689.0365000000002</v>
       </c>
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A681">
-        <v>7689.0365000000002</v>
+        <v>7696.8127000000004</v>
       </c>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A682">
-        <v>7696.8127000000004</v>
+        <v>7710.3644999999997</v>
       </c>
     </row>
     <row r="683" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A683">
-        <v>7710.3644999999997</v>
+        <v>7719.0486000000001</v>
       </c>
     </row>
     <row r="684" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A684">
-        <v>7719.0486000000001</v>
+        <v>7720.7129999999997</v>
       </c>
     </row>
     <row r="685" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A685">
-        <v>7720.7129999999997</v>
+        <v>7723.2079999999996</v>
       </c>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A686">
-        <v>7723.2079999999996</v>
+        <v>7733.7232000000004</v>
       </c>
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A687">
-        <v>7733.7232000000004</v>
+        <v>7737.6661000000004</v>
       </c>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A688">
-        <v>7737.6661000000004</v>
+        <v>7742.7047000000002</v>
       </c>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A689">
-        <v>7742.7047000000002</v>
+        <v>7745.5140000000001</v>
       </c>
     </row>
     <row r="690" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A690">
-        <v>7745.5140000000001</v>
+        <v>7746.5942999999997</v>
       </c>
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A691">
-        <v>7746.5942999999997</v>
+        <v>7748.2694000000001</v>
       </c>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A692">
-        <v>7748.2694000000001</v>
+        <v>7751.1090999999997</v>
       </c>
     </row>
     <row r="693" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A693">
-        <v>7751.1090999999997</v>
+        <v>7780.5573000000004</v>
       </c>
     </row>
     <row r="694" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A694">
-        <v>7780.5573000000004</v>
+        <v>7802.4727999999996</v>
       </c>
     </row>
     <row r="695" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A695">
-        <v>7802.4727999999996</v>
+        <v>7807.9090999999999</v>
       </c>
     </row>
     <row r="696" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A696">
-        <v>7807.9090999999999</v>
+        <v>7820.8033999999998</v>
       </c>
     </row>
     <row r="697" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A697">
-        <v>7820.8033999999998</v>
+        <v>7832.1967999999997</v>
       </c>
     </row>
     <row r="698" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A698">
-        <v>7832.1967999999997</v>
+        <v>7844.5589</v>
       </c>
     </row>
     <row r="699" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A699">
-        <v>7844.5589</v>
+        <v>7855.3987999999999</v>
       </c>
     </row>
     <row r="700" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A700">
-        <v>7855.3987999999999</v>
+        <v>7869.6106</v>
       </c>
     </row>
     <row r="701" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A701">
-        <v>7869.6106</v>
+        <v>7879.7583999999997</v>
       </c>
     </row>
     <row r="702" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A702">
-        <v>7879.7583999999997</v>
+        <v>7912.8670000000002</v>
       </c>
     </row>
     <row r="703" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A703">
-        <v>7912.8670000000002</v>
+        <v>7924.1504000000004</v>
       </c>
     </row>
     <row r="704" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A704">
-        <v>7924.1504000000004</v>
+        <v>7937.1405999999997</v>
       </c>
     </row>
     <row r="705" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A705">
-        <v>7937.1405999999997</v>
+        <v>7941.0892000000003</v>
       </c>
     </row>
     <row r="706" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A706">
-        <v>7941.0892000000003</v>
+        <v>7945.8468999999996</v>
       </c>
     </row>
     <row r="707" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A707">
-        <v>7945.8468999999996</v>
+        <v>7954.9345000000003</v>
       </c>
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A708">
-        <v>7954.9345000000003</v>
+        <v>7955.6922000000004</v>
       </c>
     </row>
     <row r="709" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A709">
-        <v>7955.6922000000004</v>
+        <v>7959.1435000000001</v>
       </c>
     </row>
     <row r="710" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A710">
-        <v>7959.1435000000001</v>
+        <v>7998.9458000000004</v>
       </c>
     </row>
     <row r="711" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A711">
-        <v>7998.9458000000004</v>
+        <v>8027.9417999999996</v>
       </c>
     </row>
     <row r="712" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A712">
-        <v>8027.9417999999996</v>
+        <v>8028.3145000000004</v>
       </c>
     </row>
     <row r="713" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A713">
-        <v>8028.3145000000004</v>
+        <v>8046.0478999999996</v>
       </c>
     </row>
     <row r="714" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A714">
-        <v>8046.0478999999996</v>
+        <v>8047.6184999999996</v>
       </c>
     </row>
     <row r="715" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A715">
-        <v>8047.6184999999996</v>
+        <v>8072.1647000000003</v>
       </c>
     </row>
     <row r="716" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A716">
-        <v>8072.1647000000003</v>
+        <v>8075.1508999999996</v>
       </c>
     </row>
     <row r="717" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A717">
-        <v>8075.1508999999996</v>
+        <v>8080.5474999999997</v>
       </c>
     </row>
     <row r="718" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A718">
-        <v>8080.5474999999997</v>
+        <v>8085.1723000000002</v>
       </c>
     </row>
     <row r="719" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A719">
-        <v>8085.1723000000002</v>
+        <v>8096.8755000000001</v>
       </c>
     </row>
     <row r="720" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A720">
-        <v>8096.8755000000001</v>
+        <v>8108.3212000000003</v>
       </c>
     </row>
     <row r="721" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A721">
-        <v>8108.3212000000003</v>
+        <v>8112.1634999999997</v>
       </c>
     </row>
     <row r="722" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A722">
-        <v>8112.1634999999997</v>
+        <v>8178.9939999999997</v>
       </c>
     </row>
     <row r="723" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A723">
-        <v>8178.9939999999997</v>
+        <v>8196.5169999999998</v>
       </c>
     </row>
     <row r="724" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A724">
-        <v>8196.5169999999998</v>
+        <v>8198.9220999999998</v>
       </c>
     </row>
     <row r="725" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A725">
-        <v>8198.9220999999998</v>
+        <v>8204.1029999999992</v>
       </c>
     </row>
     <row r="726" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A726">
-        <v>8204.1029999999992</v>
+        <v>8204.9372000000003</v>
       </c>
     </row>
     <row r="727" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A727">
-        <v>8204.9372000000003</v>
+        <v>8207.7428999999993</v>
       </c>
     </row>
     <row r="728" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A728">
-        <v>8207.7428999999993</v>
+        <v>8215.8047999999999</v>
       </c>
     </row>
     <row r="729" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A729">
-        <v>8215.8047999999999</v>
+        <v>8220.3790000000008</v>
       </c>
     </row>
     <row r="730" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A730">
-        <v>8220.3790000000008</v>
+        <v>8232.3178000000007</v>
       </c>
     </row>
     <row r="731" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A731">
-        <v>8232.3178000000007</v>
+        <v>8239.1280999999999</v>
       </c>
     </row>
     <row r="732" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A732">
-        <v>8239.1280999999999</v>
+        <v>8248.1309000000001</v>
       </c>
     </row>
     <row r="733" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A733">
-        <v>8248.1309000000001</v>
+        <v>8269.6488000000008</v>
       </c>
     </row>
     <row r="734" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A734">
-        <v>8269.6488000000008</v>
+        <v>8275.8920999999991</v>
       </c>
     </row>
     <row r="735" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A735">
-        <v>8275.8920999999991</v>
+        <v>8293.5146000000004</v>
       </c>
     </row>
     <row r="736" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A736">
-        <v>8293.5146000000004</v>
+        <v>8300.0000999999993</v>
       </c>
     </row>
     <row r="737" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A737">
-        <v>8300.0000999999993</v>
+        <v>8327.0563000000002</v>
       </c>
     </row>
     <row r="738" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A738">
-        <v>8327.0563000000002</v>
+        <v>8331.9156999999996</v>
       </c>
     </row>
     <row r="739" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A739">
-        <v>8331.9156999999996</v>
+        <v>8339.4038999999993</v>
       </c>
     </row>
     <row r="740" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A740">
-        <v>8339.4038999999993</v>
+        <v>8342.8570999999993</v>
       </c>
     </row>
     <row r="741" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A741">
-        <v>8342.8570999999993</v>
+        <v>8349.0449000000008</v>
       </c>
     </row>
     <row r="742" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A742">
-        <v>8349.0449000000008</v>
+        <v>8360.7955999999995</v>
       </c>
     </row>
     <row r="743" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A743">
-        <v>8360.7955999999995</v>
+        <v>8365.6335999999992</v>
       </c>
     </row>
     <row r="744" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A744">
-        <v>8365.6335999999992</v>
+        <v>8387.7724999999991</v>
       </c>
     </row>
     <row r="745" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A745">
-        <v>8387.7724999999991</v>
+        <v>8401.4</v>
       </c>
     </row>
     <row r="746" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A746">
-        <v>8401.4</v>
+        <v>8424.1406000000006</v>
       </c>
     </row>
     <row r="747" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A747">
-        <v>8424.1406000000006</v>
+        <v>8439.5720999999994</v>
       </c>
     </row>
     <row r="748" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A748">
-        <v>8439.5720999999994</v>
+        <v>8446.3844000000008</v>
       </c>
     </row>
     <row r="749" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A749">
-        <v>8446.3844000000008</v>
+        <v>8468.4074000000001</v>
       </c>
     </row>
     <row r="750" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A750">
-        <v>8468.4074000000001</v>
+        <v>8471.7443999999996</v>
       </c>
     </row>
     <row r="751" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A751">
-        <v>8471.7443999999996</v>
+        <v>8481.9817999999996</v>
       </c>
     </row>
     <row r="752" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A752">
-        <v>8481.9817999999996</v>
+        <v>8514.0720999999994</v>
       </c>
     </row>
     <row r="753" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A753">
-        <v>8514.0720999999994</v>
+        <v>8526.6689999999999</v>
       </c>
     </row>
     <row r="754" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A754">
-        <v>8526.6689999999999</v>
+        <v>8571.8052000000007</v>
       </c>
     </row>
     <row r="755" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A755">
-        <v>8571.8052000000007</v>
+        <v>8582.2574000000004</v>
       </c>
     </row>
     <row r="756" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A756">
-        <v>8582.2574000000004</v>
+        <v>8592.9506999999994</v>
       </c>
     </row>
     <row r="757" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A757">
-        <v>8592.9506999999994</v>
+        <v>8598.8302000000003</v>
       </c>
     </row>
     <row r="758" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A758">
-        <v>8598.8302000000003</v>
+        <v>8610.6119999999992</v>
       </c>
     </row>
     <row r="759" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A759">
-        <v>8610.6119999999992</v>
+        <v>8611.8040000000001</v>
       </c>
     </row>
     <row r="760" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A760">
-        <v>8611.8040000000001</v>
+        <v>8613.9410000000007</v>
       </c>
     </row>
     <row r="761" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A761">
-        <v>8613.9410000000007</v>
+        <v>8616.2795999999998</v>
       </c>
     </row>
     <row r="762" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A762">
-        <v>8616.2795999999998</v>
+        <v>8621.6007000000009</v>
       </c>
     </row>
     <row r="763" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A763">
-        <v>8621.6007000000009</v>
+        <v>8688.6255000000001</v>
       </c>
     </row>
     <row r="764" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A764">
-        <v>8688.6255000000001</v>
+        <v>8699.4539999999997</v>
       </c>
     </row>
     <row r="765" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A765">
-        <v>8699.4539999999997</v>
+        <v>8710.3914999999997</v>
       </c>
     </row>
     <row r="766" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A766">
-        <v>8710.3914999999997</v>
+        <v>8713.2034000000003</v>
       </c>
     </row>
     <row r="767" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A767">
-        <v>8713.2034000000003</v>
+        <v>8757.1875999999993</v>
       </c>
     </row>
     <row r="768" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A768">
-        <v>8757.1875999999993</v>
+        <v>8763.9663999999993</v>
       </c>
     </row>
     <row r="769" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A769">
-        <v>8763.9663999999993</v>
+        <v>8784.4405000000006</v>
       </c>
     </row>
     <row r="770" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A770">
-        <v>8784.4405000000006</v>
+        <v>8793.3438000000006</v>
       </c>
     </row>
     <row r="771" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A771">
-        <v>8793.3438000000006</v>
+        <v>8796.4835999999996</v>
       </c>
     </row>
     <row r="772" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A772">
-        <v>8796.4835999999996</v>
+        <v>8804.6257999999998</v>
       </c>
     </row>
     <row r="773" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A773">
-        <v>8804.6257999999998</v>
+        <v>8808.1710000000003</v>
       </c>
     </row>
     <row r="774" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A774">
-        <v>8808.1710000000003</v>
+        <v>8824.2211000000007</v>
       </c>
     </row>
     <row r="775" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A775">
-        <v>8824.2211000000007</v>
+        <v>8838.4290000000001</v>
       </c>
     </row>
     <row r="776" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A776">
-        <v>8838.4290000000001</v>
+        <v>8846.7407000000003</v>
       </c>
     </row>
     <row r="777" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A777">
-        <v>8846.7407000000003</v>
+        <v>8866.9328999999998</v>
       </c>
     </row>
     <row r="778" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A778">
-        <v>8866.9328999999998</v>
+        <v>8868.4290000000001</v>
       </c>
     </row>
     <row r="779" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A779">
-        <v>8868.4290000000001</v>
+        <v>8876.0241000000005</v>
       </c>
     </row>
     <row r="780" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A780">
-        <v>8876.0241000000005</v>
+        <v>8929.0776999999998</v>
       </c>
     </row>
     <row r="781" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A781">
-        <v>8929.0776999999998</v>
+        <v>8943.0638999999992</v>
       </c>
     </row>
     <row r="782" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A782">
-        <v>8943.0638999999992</v>
+        <v>8945.19</v>
       </c>
     </row>
     <row r="783" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A783">
-        <v>8945.19</v>
+        <v>8946.2618999999995</v>
       </c>
     </row>
     <row r="784" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A784">
-        <v>8946.2618999999995</v>
+        <v>8950.1887999999999</v>
       </c>
     </row>
     <row r="785" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A785">
-        <v>8950.1887999999999</v>
+        <v>8975.4007000000001</v>
       </c>
     </row>
     <row r="786" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A786">
-        <v>8975.4007000000001</v>
+        <v>8984.8886000000002</v>
       </c>
     </row>
     <row r="787" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A787">
-        <v>8984.8886000000002</v>
+        <v>8999.5565999999999</v>
       </c>
     </row>
     <row r="788" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A788">
-        <v>8999.5565999999999</v>
+        <v>9010.5946000000004</v>
       </c>
     </row>
     <row r="789" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A789">
-        <v>9010.5946000000004</v>
+        <v>9013.9776000000002</v>
       </c>
     </row>
     <row r="790" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A790">
-        <v>9013.9776000000002</v>
+        <v>9019.7469000000001</v>
       </c>
     </row>
     <row r="791" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A791">
-        <v>9019.7469000000001</v>
+        <v>9024.3690999999999</v>
       </c>
     </row>
     <row r="792" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A792">
-        <v>9024.3690999999999</v>
+        <v>9030.7129000000004</v>
       </c>
     </row>
     <row r="793" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A793">
-        <v>9030.7129000000004</v>
+        <v>9070.4030999999995</v>
       </c>
     </row>
     <row r="794" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A794">
-        <v>9070.4030999999995</v>
+        <v>9079.5807999999997</v>
       </c>
     </row>
     <row r="795" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A795">
-        <v>9079.5807999999997</v>
+        <v>9084.1854000000003</v>
       </c>
     </row>
     <row r="796" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A796">
-        <v>9084.1854000000003</v>
+        <v>9088.3186000000005</v>
       </c>
     </row>
     <row r="797" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A797">
-        <v>9088.3186000000005</v>
+        <v>9089.4043999999994</v>
       </c>
     </row>
     <row r="798" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A798">
-        <v>9089.4043999999994</v>
+        <v>9103.6375000000007</v>
       </c>
     </row>
     <row r="799" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A799">
-        <v>9103.6375000000007</v>
+        <v>9117.1327000000001</v>
       </c>
     </row>
     <row r="800" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A800">
-        <v>9117.1327000000001</v>
-      </c>
-    </row>
-    <row r="801" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A801">
         <v>9119.9704999999994</v>
       </c>
     </row>

</xml_diff>